<commit_message>
rename and handle env variables well
# Conflicts:
#	README.md
</commit_message>
<xml_diff>
--- a/assets/exampleFiles/report-scraper-ex.xlsx
+++ b/assets/exampleFiles/report-scraper-ex.xlsx
@@ -22,16 +22,16 @@
     <t>selector</t>
   </si>
   <si>
-    <t>lastUpdated</t>
+    <t>last-updated</t>
   </si>
   <si>
     <t>keywords</t>
   </si>
   <si>
-    <t>junkWords</t>
-  </si>
-  <si>
-    <t>clickPhrases</t>
+    <t>junk-words</t>
+  </si>
+  <si>
+    <t>click-phrases</t>
   </si>
   <si>
     <t>https://bigskyanglers.com/</t>
@@ -356,7 +356,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -366,6 +366,9 @@
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -679,11 +682,11 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="4" width="39.29071428571429" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="4" width="61.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="4" width="28.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="4" width="67.14785714285713" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="4" width="62.14785714285715" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="4" width="66.29071428571429" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="5" width="61.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="5" width="28.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="5" width="67.14785714285713" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="5" width="62.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="5" width="66.29071428571429" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">

</xml_diff>